<commit_message>
Checking in updated results
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestSBO_Replay_Monthly_RC/Model/SBO_MODEL_EVENTS_Replay_Monthly.xlsx
+++ b/src/test/resources/TestDriver/TestSBO_Replay_Monthly_RC/Model/SBO_MODEL_EVENTS_Replay_Monthly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\fyntrac-data-main\fyntrac-data-main\src\test\resources\TestDriver\TestSBO_Replay_Monthly_RC\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102CF9F-9624-4497-8A3D-A4FDA9F95E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873ADB8F-E609-4C8C-9DEE-DB844FB3CA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRANX" sheetId="27" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="85">
   <si>
     <t>Amount</t>
   </si>
@@ -1594,10 +1594,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33:G47"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1690,7 @@
         <v>44712</v>
       </c>
       <c r="B7" s="73">
-        <v>44614</v>
+        <v>44635</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
@@ -1699,12 +1699,12 @@
         <v>1</v>
       </c>
       <c r="E7" s="74">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
+      <c r="G7" s="75"/>
       <c r="H7" s="75"/>
-      <c r="I7">
+      <c r="I7" s="49">
         <v>15</v>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
         <v>44712</v>
       </c>
       <c r="B8" s="73">
-        <v>44635</v>
+        <v>44645</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>29</v>
@@ -1721,12 +1721,12 @@
       <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="74">
-        <v>1500</v>
-      </c>
-      <c r="F8" s="74"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75">
+        <v>7000</v>
+      </c>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
       <c r="I8" s="49">
         <v>15</v>
       </c>
@@ -1736,79 +1736,74 @@
         <v>44712</v>
       </c>
       <c r="B9" s="73">
-        <v>44645</v>
+        <v>44671</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="53">
         <v>1</v>
       </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="75">
-        <v>7000</v>
-      </c>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
+      <c r="E9" s="74">
+        <v>2000</v>
+      </c>
+      <c r="F9" s="74"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="49">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="72">
-        <v>44712</v>
-      </c>
-      <c r="B10" s="73">
-        <v>44671</v>
-      </c>
-      <c r="C10" s="6" t="s">
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="86" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="89">
+        <v>44651</v>
+      </c>
+      <c r="B14" s="90">
+        <v>44635</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="53">
+      <c r="D14" s="6">
         <v>1</v>
       </c>
-      <c r="E10" s="74">
-        <v>2000</v>
-      </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="49">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="83" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="84" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="81" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="86" t="s">
-        <v>30</v>
-      </c>
+      <c r="E14" s="91">
+        <v>1500</v>
+      </c>
+      <c r="F14" s="91"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="89">
         <v>44651</v>
       </c>
       <c r="B15" s="90">
-        <v>44635</v>
+        <v>44645</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>29</v>
@@ -1816,113 +1811,118 @@
       <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E15" s="91">
-        <v>1500</v>
-      </c>
-      <c r="F15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91">
+        <v>7000</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="89">
-        <v>44651</v>
+        <v>44681</v>
       </c>
       <c r="B16" s="90">
-        <v>44645</v>
+        <v>44671</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="53">
         <v>1</v>
       </c>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91">
-        <v>7000</v>
-      </c>
+      <c r="E16" s="91">
+        <v>2000</v>
+      </c>
+      <c r="F16" s="91"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="89">
-        <v>44681</v>
-      </c>
-      <c r="B17" s="90">
-        <v>44671</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="92"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+    </row>
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="83" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="76">
+        <v>44620</v>
+      </c>
+      <c r="B22" s="76">
+        <v>44620</v>
+      </c>
+      <c r="C22" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="53">
+      <c r="D22" s="69">
         <v>1</v>
       </c>
-      <c r="E17" s="91">
-        <v>2000</v>
-      </c>
-      <c r="F17" s="91"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="94"/>
-    </row>
-    <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="83" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="81" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="81" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="81" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" s="82" t="s">
-        <v>70</v>
+      <c r="E22" s="97">
+        <v>10</v>
+      </c>
+      <c r="F22" s="78">
+        <v>100000</v>
+      </c>
+      <c r="G22" s="78">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="76">
-        <v>44620</v>
-      </c>
-      <c r="B23" s="76">
-        <v>44620</v>
-      </c>
-      <c r="C23" s="69" t="s">
+      <c r="A23" s="72">
+        <v>44651</v>
+      </c>
+      <c r="B23" s="72">
+        <v>44651</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="69">
+      <c r="D23" s="6">
         <v>1</v>
       </c>
-      <c r="E23" s="97">
+      <c r="E23" s="95">
         <v>10</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="74">
         <v>100000</v>
       </c>
-      <c r="G23" s="78">
-        <v>100</v>
+      <c r="G23" s="74">
+        <v>877.77779999999996</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="72">
-        <v>44651</v>
+        <v>44681</v>
       </c>
       <c r="B24" s="72">
-        <v>44651</v>
+        <v>44681</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>29</v>
@@ -1934,92 +1934,92 @@
         <v>10</v>
       </c>
       <c r="F24" s="74">
-        <v>100000</v>
+        <v>106766.6667</v>
       </c>
       <c r="G24" s="74">
-        <v>877.77779999999996</v>
+        <v>484.73149999999998</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="72">
-        <v>44681</v>
-      </c>
-      <c r="B25" s="72">
-        <v>44681</v>
+      <c r="A25" s="96">
+        <v>44712</v>
+      </c>
+      <c r="B25" s="96">
+        <v>44712</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="53">
         <v>1</v>
       </c>
       <c r="E25" s="95">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F25" s="74">
-        <v>106766.6667</v>
+        <v>105814.88890000001</v>
       </c>
       <c r="G25" s="74">
-        <v>484.73149999999998</v>
+        <v>323.32330000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="96">
-        <v>44712</v>
-      </c>
-      <c r="B26" s="96">
-        <v>44712</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="53">
-        <v>1</v>
-      </c>
-      <c r="E26" s="95">
-        <v>15</v>
-      </c>
-      <c r="F26" s="74">
-        <v>105814.88890000001</v>
-      </c>
-      <c r="G26" s="74">
-        <v>323.32330000000002</v>
-      </c>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="112" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="114"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="112" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="113"/>
-      <c r="C29" s="113"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="113"/>
-      <c r="G29" s="113"/>
-      <c r="H29" s="114"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="100" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="98" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="98" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="98" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="100" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="F32" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G32" s="98" t="s">
-        <v>82</v>
+      <c r="A32" s="6">
+        <v>20220131</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="6">
+        <v>20220131</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="6">
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>83</v>
@@ -2042,53 +2042,53 @@
         <v>8</v>
       </c>
       <c r="G33" s="6">
-        <v>100</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <v>20220131</v>
+        <v>20220228</v>
       </c>
       <c r="B34" s="6">
         <v>1</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E34" s="6">
-        <v>20220131</v>
+        <v>20220228</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G34" s="6">
-        <v>100000</v>
+        <v>777.77779999999996</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
-        <v>20220228</v>
+        <v>20220331</v>
       </c>
       <c r="B35" s="6">
         <v>1</v>
       </c>
       <c r="C35" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="6">
-        <v>20220228</v>
+        <v>20220325</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="6">
-        <v>777.77779999999996</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2099,19 +2099,19 @@
         <v>1</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E36" s="6">
-        <v>20220325</v>
+        <v>20220315</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G36" s="6">
-        <v>7000</v>
+        <v>-1266.6667</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2122,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>84</v>
@@ -2134,7 +2134,7 @@
         <v>8</v>
       </c>
       <c r="G37" s="6">
-        <v>-1266.6667</v>
+        <v>-233.33330000000001</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2145,10 +2145,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="6">
         <v>20220315</v>
@@ -2157,7 +2157,7 @@
         <v>8</v>
       </c>
       <c r="G38" s="6">
-        <v>-233.33330000000001</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2168,42 +2168,42 @@
         <v>1</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E39" s="6">
-        <v>20220315</v>
+        <v>20220331</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G39" s="6">
-        <v>1500</v>
+        <v>873.6203999999999</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <v>20220331</v>
+        <v>20220430</v>
       </c>
       <c r="B40" s="6">
         <v>1</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E40" s="6">
-        <v>20220331</v>
+        <v>20220420</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G40" s="6">
-        <v>873.6203999999999</v>
+        <v>-1048.2221999999999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2214,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>84</v>
@@ -2226,7 +2226,7 @@
         <v>8</v>
       </c>
       <c r="G41" s="6">
-        <v>-1048.2221999999999</v>
+        <v>-951.77779999999996</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2237,10 +2237,10 @@
         <v>1</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E42" s="6">
         <v>20220420</v>
@@ -2249,7 +2249,7 @@
         <v>8</v>
       </c>
       <c r="G42" s="6">
-        <v>-951.77779999999996</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2260,42 +2260,42 @@
         <v>1</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E43" s="6">
-        <v>20220420</v>
+        <v>20220430</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G43" s="6">
-        <v>2000</v>
+        <v>886.81399999999996</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
-        <v>20220430</v>
+        <v>20220531</v>
       </c>
       <c r="B44" s="6">
         <v>1</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E44" s="6">
-        <v>20220430</v>
+        <v>20220531</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G44" s="6">
-        <v>886.81399999999996</v>
+        <v>166.7534</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>84</v>
@@ -2318,7 +2318,7 @@
         <v>8</v>
       </c>
       <c r="G45" s="6">
-        <v>164.91669999999999</v>
+        <v>1110.9444000000001</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2329,7 +2329,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>84</v>
@@ -2341,39 +2341,16 @@
         <v>8</v>
       </c>
       <c r="G46" s="6">
-        <v>710.19439999999997</v>
+        <v>1395.4749999999999</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
-        <v>20220531</v>
-      </c>
-      <c r="B47" s="6">
-        <v>1</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" s="6">
-        <v>20220531</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" s="6">
-        <v>1385.1223</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="69"/>
+      <c r="A47" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18528,10 +18505,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18613,7 +18590,7 @@
         <v>100</v>
       </c>
       <c r="I6" s="49">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -18636,26 +18613,28 @@
       <c r="G7" s="78"/>
       <c r="H7" s="79"/>
       <c r="I7" s="49">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="76">
+      <c r="A8" s="72">
         <v>44712</v>
       </c>
-      <c r="B8" s="77">
-        <v>44614</v>
-      </c>
-      <c r="C8" s="69" t="s">
+      <c r="B8" s="73">
+        <v>44635</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="69">
+      <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="79"/>
+      <c r="E8" s="74">
+        <v>1500</v>
+      </c>
+      <c r="F8" s="74"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="49">
         <v>15</v>
       </c>
@@ -18665,7 +18644,7 @@
         <v>44712</v>
       </c>
       <c r="B9" s="73">
-        <v>44635</v>
+        <v>44645</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>29</v>
@@ -18673,12 +18652,12 @@
       <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="74">
-        <v>1500</v>
-      </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75">
+        <v>7000</v>
+      </c>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="49">
         <v>15</v>
       </c>
@@ -18688,79 +18667,74 @@
         <v>44712</v>
       </c>
       <c r="B10" s="73">
-        <v>44645</v>
+        <v>44671</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="53">
         <v>1</v>
       </c>
-      <c r="E10" s="74"/>
-      <c r="F10" s="75">
-        <v>7000</v>
-      </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
+      <c r="E10" s="74">
+        <v>2000</v>
+      </c>
+      <c r="F10" s="74"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="49">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="72">
-        <v>44712</v>
-      </c>
-      <c r="B11" s="73">
-        <v>44671</v>
-      </c>
-      <c r="C11" s="6" t="s">
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="88" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="89">
+        <v>44620</v>
+      </c>
+      <c r="B15" s="89">
+        <v>44607</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="53">
+      <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E11" s="74">
-        <v>2000</v>
-      </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="49">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="83" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="84" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="88" t="s">
-        <v>30</v>
+      <c r="E15" s="101"/>
+      <c r="F15" s="91">
+        <v>5000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="89">
-        <v>44620</v>
-      </c>
-      <c r="B16" s="89">
-        <v>44607</v>
+        <v>44651</v>
+      </c>
+      <c r="B16" s="90">
+        <v>44635</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>29</v>
@@ -18768,17 +18742,17 @@
       <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="101"/>
-      <c r="F16" s="91">
-        <v>5000</v>
-      </c>
+      <c r="E16" s="91">
+        <v>1500</v>
+      </c>
+      <c r="F16" s="91"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="89">
         <v>44651</v>
       </c>
       <c r="B17" s="90">
-        <v>44635</v>
+        <v>44645</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>29</v>
@@ -18786,113 +18760,118 @@
       <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="91">
-        <v>1500</v>
-      </c>
-      <c r="F17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91">
+        <v>7000</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="89">
-        <v>44651</v>
+        <v>44681</v>
       </c>
       <c r="B18" s="90">
-        <v>44645</v>
+        <v>44671</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="53">
         <v>1</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91">
-        <v>7000</v>
-      </c>
+      <c r="E18" s="91">
+        <v>2000</v>
+      </c>
+      <c r="F18" s="91"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="89">
-        <v>44681</v>
-      </c>
-      <c r="B19" s="90">
-        <v>44671</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="A19" s="92"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+    </row>
+    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="83" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="76">
+        <v>44620</v>
+      </c>
+      <c r="B24" s="76">
+        <v>44620</v>
+      </c>
+      <c r="C24" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="53">
+      <c r="D24" s="69">
         <v>1</v>
       </c>
-      <c r="E19" s="91">
-        <v>2000</v>
-      </c>
-      <c r="F19" s="91"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-    </row>
-    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="83" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="81" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="81" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="81" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" s="82" t="s">
-        <v>70</v>
+      <c r="E24" s="97">
+        <v>10</v>
+      </c>
+      <c r="F24" s="78">
+        <v>100000</v>
+      </c>
+      <c r="G24" s="78">
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="76">
-        <v>44620</v>
-      </c>
-      <c r="B25" s="76">
-        <v>44620</v>
-      </c>
-      <c r="C25" s="69" t="s">
+      <c r="A25" s="72">
+        <v>44651</v>
+      </c>
+      <c r="B25" s="72">
+        <v>44651</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="69">
+      <c r="D25" s="6">
         <v>1</v>
       </c>
-      <c r="E25" s="97">
+      <c r="E25" s="95">
         <v>10</v>
       </c>
       <c r="F25" s="78">
-        <v>100000</v>
+        <v>105000</v>
       </c>
       <c r="G25" s="78">
-        <v>100</v>
+        <v>897.22222222222229</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="72">
-        <v>44651</v>
+        <v>44681</v>
       </c>
       <c r="B26" s="72">
-        <v>44651</v>
+        <v>44681</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>29</v>
@@ -18903,93 +18882,93 @@
       <c r="E26" s="95">
         <v>10</v>
       </c>
-      <c r="F26" s="78">
-        <v>105000</v>
-      </c>
-      <c r="G26" s="78">
-        <v>897.22222222222229</v>
+      <c r="F26" s="74">
+        <v>111805.55555555556</v>
+      </c>
+      <c r="G26" s="74">
+        <v>508.52623456790127</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="72">
-        <v>44681</v>
-      </c>
-      <c r="B27" s="72">
-        <v>44681</v>
+      <c r="A27" s="96">
+        <v>44712</v>
+      </c>
+      <c r="B27" s="96">
+        <v>44712</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="53">
         <v>1</v>
       </c>
       <c r="E27" s="95">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F27" s="74">
-        <v>111805.55555555556</v>
+        <v>110904.16666666667</v>
       </c>
       <c r="G27" s="74">
-        <v>508.52623456790127</v>
+        <v>338.87384259259261</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="96">
-        <v>44712</v>
-      </c>
-      <c r="B28" s="96">
-        <v>44712</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="53">
-        <v>1</v>
-      </c>
-      <c r="E28" s="95">
-        <v>15</v>
-      </c>
-      <c r="F28" s="74">
-        <v>110904.16666666667</v>
-      </c>
-      <c r="G28" s="74">
-        <v>338.87384259259261</v>
-      </c>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="112" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="113"/>
+      <c r="C30" s="113"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="113"/>
+      <c r="F30" s="113"/>
+      <c r="G30" s="113"/>
+      <c r="H30" s="114"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="112" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="113"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="113"/>
-      <c r="G31" s="113"/>
-      <c r="H31" s="114"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="100" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" s="98" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="98" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="98" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="100" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="F34" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G34" s="98" t="s">
-        <v>82</v>
+      <c r="A34" s="6">
+        <v>20220131</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="6">
+        <v>20220131</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="6">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -19000,7 +18979,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>83</v>
@@ -19012,30 +18991,30 @@
         <v>68</v>
       </c>
       <c r="G35" s="6">
-        <v>100</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
-        <v>20220131</v>
+        <v>20220228</v>
       </c>
       <c r="B36" s="6">
         <v>1</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
       <c r="E36" s="6">
-        <v>20220131</v>
+        <v>20220215</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G36" s="6">
-        <v>100000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -19046,42 +19025,42 @@
         <v>1</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E37" s="6">
-        <v>20220215</v>
+        <v>20220228</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G37" s="6">
-        <v>5000</v>
+        <v>797.22219999999993</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <v>20220228</v>
+        <v>20220331</v>
       </c>
       <c r="B38" s="6">
         <v>1</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="6">
-        <v>20220228</v>
+        <v>20220325</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G38" s="6">
-        <v>797.22219999999993</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -19092,19 +19071,19 @@
         <v>1</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E39" s="6">
-        <v>20220325</v>
+        <v>20220315</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G39" s="6">
-        <v>7000</v>
+        <v>-1305.5554999999999</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -19115,7 +19094,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>84</v>
@@ -19127,7 +19106,7 @@
         <v>68</v>
       </c>
       <c r="G40" s="6">
-        <v>-1305.5554999999999</v>
+        <v>-194.44450000000001</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -19138,10 +19117,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41" s="6">
         <v>20220315</v>
@@ -19150,7 +19129,7 @@
         <v>68</v>
       </c>
       <c r="G41" s="6">
-        <v>-194.44450000000001</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -19161,42 +19140,42 @@
         <v>1</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E42" s="6">
-        <v>20220315</v>
+        <v>20220331</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G42" s="6">
-        <v>1500</v>
+        <v>916.8596</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
-        <v>20220331</v>
+        <v>20220430</v>
       </c>
       <c r="B43" s="6">
         <v>1</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E43" s="6">
-        <v>20220331</v>
+        <v>20220420</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G43" s="6">
-        <v>916.8596</v>
+        <v>-1098.6112000000001</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -19207,7 +19186,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>84</v>
@@ -19219,7 +19198,7 @@
         <v>68</v>
       </c>
       <c r="G44" s="6">
-        <v>-1098.6112000000001</v>
+        <v>-901.38879999999995</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -19230,10 +19209,10 @@
         <v>1</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E45" s="6">
         <v>20220420</v>
@@ -19242,7 +19221,7 @@
         <v>68</v>
       </c>
       <c r="G45" s="6">
-        <v>-901.38879999999995</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -19253,42 +19232,42 @@
         <v>1</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E46" s="6">
-        <v>20220420</v>
+        <v>20220430</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G46" s="6">
-        <v>2000</v>
+        <v>928.95869999999991</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
-        <v>20220430</v>
+        <v>20220531</v>
       </c>
       <c r="B47" s="6">
         <v>1</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E47" s="6">
-        <v>20220430</v>
+        <v>20220531</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G47" s="6">
-        <v>928.95869999999991</v>
+        <v>233.62620000000001</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -19299,7 +19278,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>84</v>
@@ -19311,7 +19290,7 @@
         <v>68</v>
       </c>
       <c r="G48" s="6">
-        <v>233.62620000000001</v>
+        <v>1095.8333</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -19322,7 +19301,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>84</v>
@@ -19334,36 +19313,13 @@
         <v>68</v>
       </c>
       <c r="G49" s="6">
-        <v>1095.8333</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="6">
-        <v>20220531</v>
-      </c>
-      <c r="B50" s="6">
-        <v>1</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E50" s="6">
-        <v>20220531</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" s="6">
         <v>1460.8212000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>